<commit_message>
simulation template and PedrosoBatista2021 example
</commit_message>
<xml_diff>
--- a/ChaniaUrbanRoadModel/ChaniaUrbanRoadModel.xlsx
+++ b/ChaniaUrbanRoadModel/ChaniaUrbanRoadModel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leonardopedroso/Desktop/SAF model toolbox/ChaniaUrbanRoadModel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leonardopedroso/Documents/DECENTER/DECENTER-toolbox/SAFFRON/ChaniaUrbanRoadModel/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>J</t>
   </si>
@@ -95,6 +95,9 @@
   <si>
     <t># Stages</t>
   </si>
+  <si>
+    <t>Demand flow (veh/h)</t>
+  </si>
 </sst>
 </file>
 
@@ -123,7 +126,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -142,8 +145,14 @@
         <bgColor rgb="FFD9EAD3"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -361,11 +370,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -392,17 +414,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -424,17 +447,22 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -719,14 +747,14 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="24"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
@@ -790,11 +818,11 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="22"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="25"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
@@ -1078,13 +1106,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="33"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="35"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
@@ -1100,7 +1128,9 @@
       <c r="E3" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="34"/>
+      <c r="F3" s="37" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
@@ -1116,9 +1146,11 @@
         <v>1</v>
       </c>
       <c r="E4" s="6">
-        <v>15</v>
-      </c>
-      <c r="F4" s="33"/>
+        <v>5</v>
+      </c>
+      <c r="F4" s="38">
+        <v>150</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
@@ -1135,9 +1167,11 @@
         <v>2</v>
       </c>
       <c r="E5" s="6">
-        <v>50</v>
-      </c>
-      <c r="F5" s="33"/>
+        <v>26</v>
+      </c>
+      <c r="F5" s="38">
+        <v>519</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
@@ -1154,9 +1188,11 @@
         <v>1</v>
       </c>
       <c r="E6" s="6">
-        <v>5</v>
-      </c>
-      <c r="F6" s="7"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
@@ -1173,9 +1209,11 @@
         <v>2</v>
       </c>
       <c r="E7" s="6">
-        <v>45</v>
-      </c>
-      <c r="F7" s="7"/>
+        <v>11</v>
+      </c>
+      <c r="F7" s="6">
+        <v>50</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
@@ -1192,9 +1230,11 @@
         <v>1</v>
       </c>
       <c r="E8" s="6">
-        <v>3</v>
-      </c>
-      <c r="F8" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="F8" s="6">
+        <v>109</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
@@ -1211,9 +1251,11 @@
         <v>2</v>
       </c>
       <c r="E9" s="6">
-        <v>0</v>
-      </c>
-      <c r="F9" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="F9" s="6">
+        <v>106</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
@@ -1230,9 +1272,11 @@
         <v>1</v>
       </c>
       <c r="E10" s="6">
-        <v>0</v>
-      </c>
-      <c r="F10" s="7"/>
+        <v>3</v>
+      </c>
+      <c r="F10" s="6">
+        <v>39</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
@@ -1249,9 +1293,11 @@
         <v>1</v>
       </c>
       <c r="E11" s="6">
-        <v>0</v>
-      </c>
-      <c r="F11" s="7"/>
+        <v>11</v>
+      </c>
+      <c r="F11" s="6">
+        <v>39</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
@@ -1268,9 +1314,11 @@
         <v>2</v>
       </c>
       <c r="E12" s="6">
-        <v>0</v>
-      </c>
-      <c r="F12" s="7"/>
+        <v>30</v>
+      </c>
+      <c r="F12" s="6">
+        <v>6</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
@@ -1287,9 +1335,11 @@
         <v>1</v>
       </c>
       <c r="E13" s="6">
-        <v>15</v>
-      </c>
-      <c r="F13" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="F13" s="6">
+        <v>33</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
@@ -1306,9 +1356,11 @@
         <v>1</v>
       </c>
       <c r="E14" s="6">
-        <v>10</v>
-      </c>
-      <c r="F14" s="7"/>
+        <v>5</v>
+      </c>
+      <c r="F14" s="6">
+        <v>59</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
@@ -1325,9 +1377,11 @@
         <v>1</v>
       </c>
       <c r="E15" s="11">
-        <v>3</v>
-      </c>
-      <c r="F15" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="F15" s="6">
+        <v>124</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
@@ -1344,9 +1398,11 @@
         <v>3</v>
       </c>
       <c r="E16" s="11">
-        <v>0</v>
-      </c>
-      <c r="F16" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="F16" s="6">
+        <v>4</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
@@ -1363,9 +1419,11 @@
         <v>1</v>
       </c>
       <c r="E17" s="11">
-        <v>0</v>
-      </c>
-      <c r="F17" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="F17" s="6">
+        <v>6</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
@@ -1382,9 +1440,11 @@
         <v>3</v>
       </c>
       <c r="E18" s="11">
-        <v>0</v>
-      </c>
-      <c r="F18" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="F18" s="6">
+        <v>79</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
@@ -1401,9 +1461,11 @@
         <v>2</v>
       </c>
       <c r="E19" s="11">
-        <v>0</v>
-      </c>
-      <c r="F19" s="7"/>
+        <v>32</v>
+      </c>
+      <c r="F19" s="6">
+        <v>7</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
@@ -1420,9 +1482,11 @@
         <v>1</v>
       </c>
       <c r="E20" s="11">
-        <v>0</v>
-      </c>
-      <c r="F20" s="7"/>
+        <v>6</v>
+      </c>
+      <c r="F20" s="6">
+        <v>15</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
@@ -1439,9 +1503,11 @@
         <v>1</v>
       </c>
       <c r="E21" s="11">
-        <v>0</v>
-      </c>
-      <c r="F21" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="F21" s="6">
+        <v>34</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
@@ -1458,9 +1524,11 @@
         <v>2</v>
       </c>
       <c r="E22" s="11">
-        <v>0</v>
-      </c>
-      <c r="F22" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="F22" s="6">
+        <v>38</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
@@ -1477,9 +1545,11 @@
         <v>2</v>
       </c>
       <c r="E23" s="11">
-        <v>0</v>
-      </c>
-      <c r="F23" s="7"/>
+        <v>9</v>
+      </c>
+      <c r="F23" s="6">
+        <v>50</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
@@ -1496,9 +1566,11 @@
         <v>1</v>
       </c>
       <c r="E24" s="11">
-        <v>0</v>
-      </c>
-      <c r="F24" s="7"/>
+        <v>20</v>
+      </c>
+      <c r="F24" s="6">
+        <v>11</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
@@ -1515,9 +1587,11 @@
         <v>1</v>
       </c>
       <c r="E25" s="11">
-        <v>0</v>
-      </c>
-      <c r="F25" s="7"/>
+        <v>51</v>
+      </c>
+      <c r="F25" s="6">
+        <v>30</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
@@ -1534,9 +1608,11 @@
         <v>1</v>
       </c>
       <c r="E26" s="11">
-        <v>45</v>
-      </c>
-      <c r="F26" s="7"/>
+        <v>11</v>
+      </c>
+      <c r="F26" s="6">
+        <v>143</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
@@ -1553,9 +1629,11 @@
         <v>1</v>
       </c>
       <c r="E27" s="11">
-        <v>0</v>
-      </c>
-      <c r="F27" s="7"/>
+        <v>15</v>
+      </c>
+      <c r="F27" s="6">
+        <v>30</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
@@ -1572,9 +1650,11 @@
         <v>1</v>
       </c>
       <c r="E28" s="11">
-        <v>0</v>
-      </c>
-      <c r="F28" s="7"/>
+        <v>18</v>
+      </c>
+      <c r="F28" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
@@ -1591,9 +1671,11 @@
         <v>2</v>
       </c>
       <c r="E29" s="11">
-        <v>70</v>
-      </c>
-      <c r="F29" s="7"/>
+        <v>43</v>
+      </c>
+      <c r="F29" s="6">
+        <v>388</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
@@ -1610,9 +1692,11 @@
         <v>1</v>
       </c>
       <c r="E30" s="11">
-        <v>0</v>
-      </c>
-      <c r="F30" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="F30" s="6">
+        <v>27</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
@@ -1629,9 +1713,11 @@
         <v>1</v>
       </c>
       <c r="E31" s="11">
-        <v>0</v>
-      </c>
-      <c r="F31" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="F31" s="6">
+        <v>36</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
@@ -1648,9 +1734,11 @@
         <v>2</v>
       </c>
       <c r="E32" s="11">
-        <v>0</v>
-      </c>
-      <c r="F32" s="7"/>
+        <v>9</v>
+      </c>
+      <c r="F32" s="6">
+        <v>54</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
@@ -1667,9 +1755,11 @@
         <v>1</v>
       </c>
       <c r="E33" s="11">
-        <v>0</v>
-      </c>
-      <c r="F33" s="7"/>
+        <v>26</v>
+      </c>
+      <c r="F33" s="6">
+        <v>9</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
@@ -1686,9 +1776,11 @@
         <v>1</v>
       </c>
       <c r="E34" s="11">
-        <v>0</v>
-      </c>
-      <c r="F34" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="F34" s="6">
+        <v>25</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
@@ -1705,9 +1797,11 @@
         <v>1</v>
       </c>
       <c r="E35" s="11">
-        <v>0</v>
-      </c>
-      <c r="F35" s="7"/>
+        <v>9</v>
+      </c>
+      <c r="F35" s="6">
+        <v>4</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
@@ -1724,9 +1818,11 @@
         <v>2</v>
       </c>
       <c r="E36" s="11">
-        <v>45</v>
-      </c>
-      <c r="F36" s="7"/>
+        <v>39</v>
+      </c>
+      <c r="F36" s="6">
+        <v>302</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
@@ -1743,9 +1839,11 @@
         <v>1</v>
       </c>
       <c r="E37" s="11">
-        <v>13</v>
-      </c>
-      <c r="F37" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="F37" s="6">
+        <v>247</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
@@ -1762,9 +1860,11 @@
         <v>1</v>
       </c>
       <c r="E38" s="11">
-        <v>18</v>
-      </c>
-      <c r="F38" s="7"/>
+        <v>13</v>
+      </c>
+      <c r="F38" s="6">
+        <v>74</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
@@ -1781,9 +1881,11 @@
         <v>1</v>
       </c>
       <c r="E39" s="11">
-        <v>15</v>
-      </c>
-      <c r="F39" s="7"/>
+        <v>5</v>
+      </c>
+      <c r="F39" s="6">
+        <v>281</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
@@ -1800,9 +1902,11 @@
         <v>1</v>
       </c>
       <c r="E40" s="11">
-        <v>0</v>
-      </c>
-      <c r="F40" s="7"/>
+        <v>30</v>
+      </c>
+      <c r="F40" s="6">
+        <v>16</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
@@ -1819,9 +1923,11 @@
         <v>1</v>
       </c>
       <c r="E41" s="11">
-        <v>0</v>
-      </c>
-      <c r="F41" s="7"/>
+        <v>24</v>
+      </c>
+      <c r="F41" s="6">
+        <v>40</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
@@ -1840,7 +1946,9 @@
       <c r="E42" s="11">
         <v>0</v>
       </c>
-      <c r="F42" s="7"/>
+      <c r="F42" s="6">
+        <v>9</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
@@ -1857,9 +1965,11 @@
         <v>3</v>
       </c>
       <c r="E43" s="11">
-        <v>0</v>
-      </c>
-      <c r="F43" s="7"/>
+        <v>11</v>
+      </c>
+      <c r="F43" s="6">
+        <v>26</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
@@ -1876,9 +1986,11 @@
         <v>2</v>
       </c>
       <c r="E44" s="11">
-        <v>20</v>
-      </c>
-      <c r="F44" s="7"/>
+        <v>18</v>
+      </c>
+      <c r="F44" s="6">
+        <v>197</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
@@ -1895,9 +2007,11 @@
         <v>3</v>
       </c>
       <c r="E45" s="11">
-        <v>0</v>
-      </c>
-      <c r="F45" s="7"/>
+        <v>12</v>
+      </c>
+      <c r="F45" s="6">
+        <v>12</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
@@ -1914,9 +2028,11 @@
         <v>1</v>
       </c>
       <c r="E46" s="11">
-        <v>0</v>
-      </c>
-      <c r="F46" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="F46" s="6">
+        <v>1</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
@@ -1933,9 +2049,11 @@
         <v>1</v>
       </c>
       <c r="E47" s="11">
-        <v>0</v>
-      </c>
-      <c r="F47" s="7"/>
+        <v>12</v>
+      </c>
+      <c r="F47" s="6">
+        <v>24</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
@@ -1952,9 +2070,11 @@
         <v>1</v>
       </c>
       <c r="E48" s="11">
-        <v>0</v>
-      </c>
-      <c r="F48" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="F48" s="6">
+        <v>8</v>
+      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
@@ -1971,9 +2091,11 @@
         <v>1</v>
       </c>
       <c r="E49" s="11">
-        <v>10</v>
-      </c>
-      <c r="F49" s="7"/>
+        <v>6</v>
+      </c>
+      <c r="F49" s="6">
+        <v>148</v>
+      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
@@ -1990,9 +2112,11 @@
         <v>1</v>
       </c>
       <c r="E50" s="11">
-        <v>0</v>
-      </c>
-      <c r="F50" s="7"/>
+        <v>27</v>
+      </c>
+      <c r="F50" s="6">
+        <v>12</v>
+      </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
@@ -2009,9 +2133,11 @@
         <v>1</v>
       </c>
       <c r="E51" s="11">
-        <v>0</v>
-      </c>
-      <c r="F51" s="7"/>
+        <v>9</v>
+      </c>
+      <c r="F51" s="6">
+        <v>18</v>
+      </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
@@ -2028,9 +2154,11 @@
         <v>1</v>
       </c>
       <c r="E52" s="11">
-        <v>4</v>
-      </c>
-      <c r="F52" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="F52" s="6">
+        <v>134</v>
+      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
@@ -2047,9 +2175,11 @@
         <v>1</v>
       </c>
       <c r="E53" s="11">
-        <v>10</v>
-      </c>
-      <c r="F53" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="F53" s="6">
+        <v>100</v>
+      </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
@@ -2066,9 +2196,11 @@
         <v>1</v>
       </c>
       <c r="E54" s="11">
-        <v>0</v>
-      </c>
-      <c r="F54" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="F54" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
@@ -2085,9 +2217,11 @@
         <v>1</v>
       </c>
       <c r="E55" s="11">
-        <v>0</v>
-      </c>
-      <c r="F55" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="F55" s="6">
+        <v>21</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
@@ -2104,9 +2238,11 @@
         <v>1</v>
       </c>
       <c r="E56" s="11">
-        <v>10</v>
-      </c>
-      <c r="F56" s="7"/>
+        <v>3</v>
+      </c>
+      <c r="F56" s="6">
+        <v>90</v>
+      </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
@@ -2123,9 +2259,11 @@
         <v>1</v>
       </c>
       <c r="E57" s="11">
-        <v>10</v>
-      </c>
-      <c r="F57" s="7"/>
+        <v>3</v>
+      </c>
+      <c r="F57" s="6">
+        <v>285</v>
+      </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
@@ -2142,9 +2280,11 @@
         <v>1</v>
       </c>
       <c r="E58" s="11">
-        <v>8</v>
-      </c>
-      <c r="F58" s="7"/>
+        <v>5</v>
+      </c>
+      <c r="F58" s="6">
+        <v>128</v>
+      </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="4">
@@ -2161,9 +2301,11 @@
         <v>1</v>
       </c>
       <c r="E59" s="11">
-        <v>0</v>
-      </c>
-      <c r="F59" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="F59" s="6">
+        <v>5</v>
+      </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
@@ -2180,9 +2322,11 @@
         <v>1</v>
       </c>
       <c r="E60" s="11">
-        <v>0</v>
-      </c>
-      <c r="F60" s="7"/>
+        <v>7</v>
+      </c>
+      <c r="F60" s="6">
+        <v>21</v>
+      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="4">
@@ -2199,9 +2343,11 @@
         <v>1</v>
       </c>
       <c r="E61" s="11">
-        <v>0</v>
-      </c>
-      <c r="F61" s="7"/>
+        <v>2</v>
+      </c>
+      <c r="F61" s="6">
+        <v>25</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="4">
@@ -2218,9 +2364,11 @@
         <v>1</v>
       </c>
       <c r="E62" s="11">
-        <v>60</v>
-      </c>
-      <c r="F62" s="7"/>
+        <v>28</v>
+      </c>
+      <c r="F62" s="6">
+        <v>349</v>
+      </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="4">
@@ -2237,13 +2385,15 @@
         <v>1</v>
       </c>
       <c r="E63" s="11">
-        <v>30</v>
-      </c>
-      <c r="F63" s="7"/>
+        <v>17</v>
+      </c>
+      <c r="F63" s="6">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2271,97 +2421,97 @@
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A2" s="10"/>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="25"/>
-      <c r="T2" s="25"/>
-      <c r="U2" s="25"/>
-      <c r="V2" s="25"/>
-      <c r="W2" s="25"/>
-      <c r="X2" s="25"/>
-      <c r="Y2" s="25"/>
-      <c r="Z2" s="25"/>
-      <c r="AA2" s="25"/>
-      <c r="AB2" s="25"/>
-      <c r="AC2" s="25"/>
-      <c r="AD2" s="25"/>
-      <c r="AE2" s="25"/>
-      <c r="AF2" s="25"/>
-      <c r="AG2" s="25"/>
-      <c r="AH2" s="25"/>
-      <c r="AI2" s="25"/>
-      <c r="AJ2" s="25"/>
-      <c r="AK2" s="25"/>
-      <c r="AL2" s="25"/>
-      <c r="AM2" s="25"/>
-      <c r="AN2" s="25"/>
-      <c r="AO2" s="25"/>
-      <c r="AP2" s="25"/>
-      <c r="AQ2" s="25"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="26"/>
+      <c r="U2" s="26"/>
+      <c r="V2" s="26"/>
+      <c r="W2" s="26"/>
+      <c r="X2" s="26"/>
+      <c r="Y2" s="26"/>
+      <c r="Z2" s="26"/>
+      <c r="AA2" s="26"/>
+      <c r="AB2" s="26"/>
+      <c r="AC2" s="26"/>
+      <c r="AD2" s="26"/>
+      <c r="AE2" s="26"/>
+      <c r="AF2" s="26"/>
+      <c r="AG2" s="26"/>
+      <c r="AH2" s="26"/>
+      <c r="AI2" s="26"/>
+      <c r="AJ2" s="26"/>
+      <c r="AK2" s="26"/>
+      <c r="AL2" s="26"/>
+      <c r="AM2" s="26"/>
+      <c r="AN2" s="26"/>
+      <c r="AO2" s="26"/>
+      <c r="AP2" s="26"/>
+      <c r="AQ2" s="26"/>
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A3" s="10"/>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="26"/>
-      <c r="S3" s="26"/>
-      <c r="T3" s="26"/>
-      <c r="U3" s="26"/>
-      <c r="V3" s="26"/>
-      <c r="W3" s="26"/>
-      <c r="X3" s="26"/>
-      <c r="Y3" s="26"/>
-      <c r="Z3" s="26"/>
-      <c r="AA3" s="26"/>
-      <c r="AB3" s="26"/>
-      <c r="AC3" s="26"/>
-      <c r="AD3" s="26"/>
-      <c r="AE3" s="26"/>
-      <c r="AF3" s="26"/>
-      <c r="AG3" s="26"/>
-      <c r="AH3" s="26"/>
-      <c r="AI3" s="26"/>
-      <c r="AJ3" s="26"/>
-      <c r="AK3" s="26"/>
-      <c r="AL3" s="26"/>
-      <c r="AM3" s="26"/>
-      <c r="AN3" s="26"/>
-      <c r="AO3" s="26"/>
-      <c r="AP3" s="26"/>
-      <c r="AQ3" s="26"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="27"/>
+      <c r="R3" s="27"/>
+      <c r="S3" s="27"/>
+      <c r="T3" s="27"/>
+      <c r="U3" s="27"/>
+      <c r="V3" s="27"/>
+      <c r="W3" s="27"/>
+      <c r="X3" s="27"/>
+      <c r="Y3" s="27"/>
+      <c r="Z3" s="27"/>
+      <c r="AA3" s="27"/>
+      <c r="AB3" s="27"/>
+      <c r="AC3" s="27"/>
+      <c r="AD3" s="27"/>
+      <c r="AE3" s="27"/>
+      <c r="AF3" s="27"/>
+      <c r="AG3" s="27"/>
+      <c r="AH3" s="27"/>
+      <c r="AI3" s="27"/>
+      <c r="AJ3" s="27"/>
+      <c r="AK3" s="27"/>
+      <c r="AL3" s="27"/>
+      <c r="AM3" s="27"/>
+      <c r="AN3" s="27"/>
+      <c r="AO3" s="27"/>
+      <c r="AP3" s="27"/>
+      <c r="AQ3" s="27"/>
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
@@ -10489,134 +10639,134 @@
     </row>
     <row r="2" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A2" s="10"/>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="31"/>
-      <c r="V2" s="31"/>
-      <c r="W2" s="31"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="31"/>
-      <c r="Z2" s="31"/>
-      <c r="AA2" s="31"/>
-      <c r="AB2" s="31"/>
-      <c r="AC2" s="31"/>
-      <c r="AD2" s="31"/>
-      <c r="AE2" s="31"/>
-      <c r="AF2" s="31"/>
-      <c r="AG2" s="31"/>
-      <c r="AH2" s="31"/>
-      <c r="AI2" s="31"/>
-      <c r="AJ2" s="31"/>
-      <c r="AK2" s="31"/>
-      <c r="AL2" s="31"/>
-      <c r="AM2" s="31"/>
-      <c r="AN2" s="31"/>
-      <c r="AO2" s="31"/>
-      <c r="AP2" s="31"/>
-      <c r="AQ2" s="31"/>
-      <c r="AR2" s="31"/>
-      <c r="AS2" s="31"/>
-      <c r="AT2" s="31"/>
-      <c r="AU2" s="31"/>
-      <c r="AV2" s="31"/>
-      <c r="AW2" s="31"/>
-      <c r="AX2" s="31"/>
-      <c r="AY2" s="31"/>
-      <c r="AZ2" s="31"/>
-      <c r="BA2" s="31"/>
-      <c r="BB2" s="31"/>
-      <c r="BC2" s="31"/>
-      <c r="BD2" s="31"/>
-      <c r="BE2" s="31"/>
-      <c r="BF2" s="31"/>
-      <c r="BG2" s="31"/>
-      <c r="BH2" s="31"/>
-      <c r="BI2" s="31"/>
-      <c r="BJ2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="32"/>
+      <c r="AA2" s="32"/>
+      <c r="AB2" s="32"/>
+      <c r="AC2" s="32"/>
+      <c r="AD2" s="32"/>
+      <c r="AE2" s="32"/>
+      <c r="AF2" s="32"/>
+      <c r="AG2" s="32"/>
+      <c r="AH2" s="32"/>
+      <c r="AI2" s="32"/>
+      <c r="AJ2" s="32"/>
+      <c r="AK2" s="32"/>
+      <c r="AL2" s="32"/>
+      <c r="AM2" s="32"/>
+      <c r="AN2" s="32"/>
+      <c r="AO2" s="32"/>
+      <c r="AP2" s="32"/>
+      <c r="AQ2" s="32"/>
+      <c r="AR2" s="32"/>
+      <c r="AS2" s="32"/>
+      <c r="AT2" s="32"/>
+      <c r="AU2" s="32"/>
+      <c r="AV2" s="32"/>
+      <c r="AW2" s="32"/>
+      <c r="AX2" s="32"/>
+      <c r="AY2" s="32"/>
+      <c r="AZ2" s="32"/>
+      <c r="BA2" s="32"/>
+      <c r="BB2" s="32"/>
+      <c r="BC2" s="32"/>
+      <c r="BD2" s="32"/>
+      <c r="BE2" s="32"/>
+      <c r="BF2" s="32"/>
+      <c r="BG2" s="32"/>
+      <c r="BH2" s="32"/>
+      <c r="BI2" s="32"/>
+      <c r="BJ2" s="20"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A3" s="10"/>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="28"/>
-      <c r="P3" s="28"/>
-      <c r="Q3" s="28"/>
-      <c r="R3" s="28"/>
-      <c r="S3" s="28"/>
-      <c r="T3" s="28"/>
-      <c r="U3" s="28"/>
-      <c r="V3" s="28"/>
-      <c r="W3" s="28"/>
-      <c r="X3" s="28"/>
-      <c r="Y3" s="28"/>
-      <c r="Z3" s="28"/>
-      <c r="AA3" s="28"/>
-      <c r="AB3" s="28"/>
-      <c r="AC3" s="28"/>
-      <c r="AD3" s="28"/>
-      <c r="AE3" s="28"/>
-      <c r="AF3" s="28"/>
-      <c r="AG3" s="28"/>
-      <c r="AH3" s="28"/>
-      <c r="AI3" s="28"/>
-      <c r="AJ3" s="28"/>
-      <c r="AK3" s="28"/>
-      <c r="AL3" s="28"/>
-      <c r="AM3" s="28"/>
-      <c r="AN3" s="28"/>
-      <c r="AO3" s="28"/>
-      <c r="AP3" s="28"/>
-      <c r="AQ3" s="28"/>
-      <c r="AR3" s="28"/>
-      <c r="AS3" s="28"/>
-      <c r="AT3" s="28"/>
-      <c r="AU3" s="28"/>
-      <c r="AV3" s="28"/>
-      <c r="AW3" s="28"/>
-      <c r="AX3" s="28"/>
-      <c r="AY3" s="28"/>
-      <c r="AZ3" s="28"/>
-      <c r="BA3" s="28"/>
-      <c r="BB3" s="28"/>
-      <c r="BC3" s="28"/>
-      <c r="BD3" s="28"/>
-      <c r="BE3" s="28"/>
-      <c r="BF3" s="28"/>
-      <c r="BG3" s="28"/>
-      <c r="BH3" s="28"/>
-      <c r="BI3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
+      <c r="T3" s="29"/>
+      <c r="U3" s="29"/>
+      <c r="V3" s="29"/>
+      <c r="W3" s="29"/>
+      <c r="X3" s="29"/>
+      <c r="Y3" s="29"/>
+      <c r="Z3" s="29"/>
+      <c r="AA3" s="29"/>
+      <c r="AB3" s="29"/>
+      <c r="AC3" s="29"/>
+      <c r="AD3" s="29"/>
+      <c r="AE3" s="29"/>
+      <c r="AF3" s="29"/>
+      <c r="AG3" s="29"/>
+      <c r="AH3" s="29"/>
+      <c r="AI3" s="29"/>
+      <c r="AJ3" s="29"/>
+      <c r="AK3" s="29"/>
+      <c r="AL3" s="29"/>
+      <c r="AM3" s="29"/>
+      <c r="AN3" s="29"/>
+      <c r="AO3" s="29"/>
+      <c r="AP3" s="29"/>
+      <c r="AQ3" s="29"/>
+      <c r="AR3" s="29"/>
+      <c r="AS3" s="29"/>
+      <c r="AT3" s="29"/>
+      <c r="AU3" s="29"/>
+      <c r="AV3" s="29"/>
+      <c r="AW3" s="29"/>
+      <c r="AX3" s="29"/>
+      <c r="AY3" s="29"/>
+      <c r="AZ3" s="29"/>
+      <c r="BA3" s="29"/>
+      <c r="BB3" s="29"/>
+      <c r="BC3" s="29"/>
+      <c r="BD3" s="29"/>
+      <c r="BE3" s="29"/>
+      <c r="BF3" s="29"/>
+      <c r="BG3" s="29"/>
+      <c r="BH3" s="29"/>
+      <c r="BI3" s="30"/>
       <c r="BJ3" s="16" t="s">
         <v>18</v>
       </c>

</xml_diff>